<commit_message>
Updated code with daily reports, updated leave requisition code, adding smaxtransaction table for attendance
</commit_message>
<xml_diff>
--- a/ExcelTemplates/Employee Import.xlsx
+++ b/ExcelTemplates/Employee Import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manishankar.ts\source\repos\AttendanceSystem_API\ExcelTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\internship041\source\repos\BackendFrontendAttendance\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966A2ECB-479D-4B03-8C35-70CC5496CDA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B2A14B-483D-45DF-BB5E-1585F52EC79E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{666D5FB0-F1AA-44ED-AFDF-02A18A1E0DC9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>CardCode</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>StaffId</t>
   </si>
 </sst>
 </file>
@@ -591,309 +594,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD06EFBD-18CC-421B-A80E-0C8F65DB802F}">
-  <dimension ref="A1:BS2"/>
+  <dimension ref="A1:BT2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BT8" sqref="BT8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="25" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="14" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="17" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="11" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="14" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="17" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="11" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="25" bestFit="1" customWidth="1"/>
+    <col min="62" max="63" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="14" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="17" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="14" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="17" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>57</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>59</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>60</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>61</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>62</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>63</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>64</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>24</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>25</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>28</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>33</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>65</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>69</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>70</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>66</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>67</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>34</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>35</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>36</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>37</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>38</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>39</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>40</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>41</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>42</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>43</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>44</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>45</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>46</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>47</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>48</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>49</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>50</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>51</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>68</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>52</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>53</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>54</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>55</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="L2" s="1"/>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
       <c r="M2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="AQ2" s="2"/>
-      <c r="AS2" s="2"/>
+      <c r="N2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="AR2" s="2"/>
+      <c r="AT2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>